<commit_message>
Add SO1-1 summary table
</commit_message>
<xml_diff>
--- a/LDMP/data/summary_table_ldn_sdg.xlsx
+++ b/LDMP/data/summary_table_ldn_sdg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\LandDegradation\trends.earth\LDMP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16B68D9-C4AD-4388-963F-E34F3CD63FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE48CE29-C227-4B0F-BE88-099FA336E023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="28800" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SDG 15.3.1" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Soil organic carbon" sheetId="7" r:id="rId3"/>
     <sheet name="Land cover" sheetId="8" r:id="rId4"/>
     <sheet name="Population" sheetId="9" r:id="rId5"/>
+    <sheet name="UNCCD SO1-1" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="98">
   <si>
     <t>Land area with improved productivity:</t>
   </si>
@@ -247,17 +248,100 @@
   </si>
   <si>
     <t>Degraded land:</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Artificial surfaces</t>
+  </si>
+  <si>
+    <t>Other Lands</t>
+  </si>
+  <si>
+    <t>Percent of total land area (%)</t>
+  </si>
+  <si>
+    <t>Land area with degraded land cover</t>
+  </si>
+  <si>
+    <t>Land area with no land cover data</t>
+  </si>
+  <si>
+    <t>Land area with stable land cover</t>
+  </si>
+  <si>
+    <t>Land area with improved land cover</t>
+  </si>
+  <si>
+    <t>Land area with non-degraded land cover</t>
+  </si>
+  <si>
+    <t>Total area</t>
+  </si>
+  <si>
+    <t>Estimates of land cover change (in sq km) for the baseline period (form SO1-1.T6 on UNCCD Prais system)</t>
+  </si>
+  <si>
+    <t>Estimates of land cover change (in sq km) for the progress period (UNCCD form SO1-1.T7 on Prais)</t>
+  </si>
+  <si>
+    <t>Estimates of land cover degradation (sq km) in the baseline period (form SO1-1.T8 on UNCCD Prais system)</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Estimates of land cover degradation (sq km) in the progress period (form SO1-1.T8 on UNCCD Prais system)</t>
+  </si>
+  <si>
+    <t>Trends.Earth summary table (aligned with UNCCD reporting for Strategic Objective 1)</t>
+  </si>
+  <si>
+    <t>Estimates of land cover (sq km) for the baseline period</t>
+  </si>
+  <si>
+    <t>Tree-covered areas (sq km)</t>
+  </si>
+  <si>
+    <t>Grasslands (sq km)</t>
+  </si>
+  <si>
+    <t>Croplands (sq km)</t>
+  </si>
+  <si>
+    <t>Wetlands (sq km)</t>
+  </si>
+  <si>
+    <t>Other Lands (sq km)</t>
+  </si>
+  <si>
+    <t>Water bodies (sq km)</t>
+  </si>
+  <si>
+    <t>No data (sq km)</t>
+  </si>
+  <si>
+    <t>Estimates of land cover (sq km) for the progress period</t>
+  </si>
+  <si>
+    <t>Artificial surfaces
+(sq km)</t>
+  </si>
+  <si>
+    <t>Trends in land cover (UNCCD SO1-1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,6 +485,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF27272A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF27272A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -482,7 +608,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -687,13 +813,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -916,29 +1080,52 @@
     <xf numFmtId="10" fontId="9" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="8" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="8" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="13" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="13" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="9" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="9" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -952,6 +1139,12 @@
     <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -980,6 +1173,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1012,49 +1212,557 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="9" fillId="8" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="8" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="9" fillId="13" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="13" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="9" fillId="9" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="9" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{1B5C13A4-9274-4736-9A1E-C99559450C60}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="54">
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC71BC7"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1407,18 +2115,18 @@
       <c r="A2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
     </row>
     <row r="4" spans="1:10" s="39" customFormat="1" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="41"/>
@@ -1501,18 +2209,18 @@
       <c r="A10" s="4"/>
     </row>
     <row r="11" spans="1:10" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="85" t="s">
+      <c r="A11" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="85"/>
-      <c r="C11" s="85"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="85"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="85"/>
-      <c r="I11" s="85"/>
-      <c r="J11" s="85"/>
+      <c r="B11" s="97"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="97"/>
+      <c r="H11" s="97"/>
+      <c r="I11" s="97"/>
+      <c r="J11" s="97"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
@@ -1553,18 +2261,18 @@
       <c r="A2" s="4"/>
     </row>
     <row r="3" spans="1:10" s="52" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -1645,18 +2353,18 @@
       <c r="J10" s="51"/>
     </row>
     <row r="11" spans="1:10" s="52" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="85" t="s">
+      <c r="A11" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="88"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="88"/>
+      <c r="B11" s="120"/>
+      <c r="C11" s="120"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="120"/>
+      <c r="G11" s="120"/>
+      <c r="H11" s="120"/>
+      <c r="I11" s="120"/>
+      <c r="J11" s="120"/>
     </row>
     <row r="12" spans="1:10" s="52" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
@@ -1670,30 +2378,30 @@
       <c r="J12" s="51"/>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="86" t="s">
+      <c r="A13" s="119" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
+      <c r="B13" s="119"/>
+      <c r="C13" s="119"/>
+      <c r="D13" s="119"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
+      <c r="G13" s="119"/>
+      <c r="H13" s="119"/>
+      <c r="I13" s="119"/>
+      <c r="J13" s="119"/>
     </row>
     <row r="14" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="89" t="s">
+      <c r="C14" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="90"/>
-      <c r="I14" s="90"/>
+      <c r="D14" s="106"/>
+      <c r="E14" s="106"/>
+      <c r="F14" s="106"/>
+      <c r="G14" s="106"/>
+      <c r="H14" s="106"/>
+      <c r="I14" s="106"/>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C15" s="62" t="s">
@@ -1722,7 +2430,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="91" t="s">
+      <c r="A16" s="98" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="59" t="s">
@@ -1741,7 +2449,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="87"/>
+      <c r="A17" s="99"/>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
@@ -1758,7 +2466,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="87"/>
+      <c r="A18" s="99"/>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1775,7 +2483,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="87"/>
+      <c r="A19" s="99"/>
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
@@ -1792,7 +2500,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="87"/>
+      <c r="A20" s="99"/>
       <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
@@ -1809,7 +2517,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="87"/>
+      <c r="A21" s="99"/>
       <c r="B21" s="2" t="s">
         <v>48</v>
       </c>
@@ -1826,7 +2534,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="87"/>
+      <c r="A22" s="99"/>
       <c r="B22" s="2" t="s">
         <v>9</v>
       </c>
@@ -1881,30 +2589,30 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="92" t="s">
+      <c r="A25" s="121" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="92"/>
-      <c r="C25" s="92"/>
-      <c r="D25" s="92"/>
-      <c r="E25" s="92"/>
-      <c r="F25" s="92"/>
-      <c r="G25" s="92"/>
-      <c r="H25" s="92"/>
-      <c r="I25" s="92"/>
-      <c r="J25" s="92"/>
+      <c r="B25" s="121"/>
+      <c r="C25" s="121"/>
+      <c r="D25" s="121"/>
+      <c r="E25" s="121"/>
+      <c r="F25" s="121"/>
+      <c r="G25" s="121"/>
+      <c r="H25" s="121"/>
+      <c r="I25" s="121"/>
+      <c r="J25" s="121"/>
     </row>
     <row r="26" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
-      <c r="C26" s="89" t="s">
+      <c r="C26" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="90"/>
-      <c r="E26" s="90"/>
-      <c r="F26" s="90"/>
-      <c r="G26" s="90"/>
-      <c r="H26" s="90"/>
-      <c r="I26" s="90"/>
+      <c r="D26" s="106"/>
+      <c r="E26" s="106"/>
+      <c r="F26" s="106"/>
+      <c r="G26" s="106"/>
+      <c r="H26" s="106"/>
+      <c r="I26" s="106"/>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C27" s="61" t="s">
@@ -1933,7 +2641,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="91" t="s">
+      <c r="A28" s="98" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="59" t="s">
@@ -1952,7 +2660,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="87"/>
+      <c r="A29" s="99"/>
       <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
@@ -1969,7 +2677,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="87"/>
+      <c r="A30" s="99"/>
       <c r="B30" s="2" t="s">
         <v>6</v>
       </c>
@@ -1986,7 +2694,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="87"/>
+      <c r="A31" s="99"/>
       <c r="B31" s="2" t="s">
         <v>7</v>
       </c>
@@ -2003,7 +2711,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="87"/>
+      <c r="A32" s="99"/>
       <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
@@ -2020,7 +2728,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="87"/>
+      <c r="A33" s="99"/>
       <c r="B33" s="2" t="s">
         <v>48</v>
       </c>
@@ -2037,7 +2745,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="87"/>
+      <c r="A34" s="99"/>
       <c r="B34" s="2" t="s">
         <v>9</v>
       </c>
@@ -2092,30 +2800,30 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="94" t="s">
+      <c r="A37" s="101" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="95"/>
-      <c r="C37" s="96"/>
-      <c r="D37" s="96"/>
-      <c r="E37" s="96"/>
-      <c r="F37" s="96"/>
-      <c r="G37" s="96"/>
-      <c r="H37" s="96"/>
-      <c r="I37" s="96"/>
-      <c r="J37" s="97"/>
+      <c r="B37" s="102"/>
+      <c r="C37" s="103"/>
+      <c r="D37" s="103"/>
+      <c r="E37" s="103"/>
+      <c r="F37" s="103"/>
+      <c r="G37" s="103"/>
+      <c r="H37" s="103"/>
+      <c r="I37" s="103"/>
+      <c r="J37" s="104"/>
     </row>
     <row r="38" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
-      <c r="C38" s="89" t="s">
+      <c r="C38" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="90"/>
-      <c r="E38" s="90"/>
-      <c r="F38" s="90"/>
-      <c r="G38" s="90"/>
-      <c r="H38" s="90"/>
-      <c r="I38" s="90"/>
+      <c r="D38" s="106"/>
+      <c r="E38" s="106"/>
+      <c r="F38" s="106"/>
+      <c r="G38" s="106"/>
+      <c r="H38" s="106"/>
+      <c r="I38" s="106"/>
     </row>
     <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C39" s="61" t="s">
@@ -2144,7 +2852,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="91" t="s">
+      <c r="A40" s="98" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="59" t="s">
@@ -2163,7 +2871,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="87"/>
+      <c r="A41" s="99"/>
       <c r="B41" s="2" t="s">
         <v>5</v>
       </c>
@@ -2180,7 +2888,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="87"/>
+      <c r="A42" s="99"/>
       <c r="B42" s="2" t="s">
         <v>6</v>
       </c>
@@ -2197,7 +2905,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="87"/>
+      <c r="A43" s="99"/>
       <c r="B43" s="2" t="s">
         <v>7</v>
       </c>
@@ -2214,7 +2922,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="87"/>
+      <c r="A44" s="99"/>
       <c r="B44" s="2" t="s">
         <v>8</v>
       </c>
@@ -2231,7 +2939,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="87"/>
+      <c r="A45" s="99"/>
       <c r="B45" s="2" t="s">
         <v>48</v>
       </c>
@@ -2248,7 +2956,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="87"/>
+      <c r="A46" s="99"/>
       <c r="B46" s="2" t="s">
         <v>9</v>
       </c>
@@ -2303,30 +3011,30 @@
       </c>
     </row>
     <row r="49" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="98" t="s">
+      <c r="A49" s="107" t="s">
         <v>59</v>
       </c>
-      <c r="B49" s="99"/>
-      <c r="C49" s="100"/>
-      <c r="D49" s="100"/>
-      <c r="E49" s="100"/>
-      <c r="F49" s="100"/>
-      <c r="G49" s="100"/>
-      <c r="H49" s="100"/>
-      <c r="I49" s="100"/>
-      <c r="J49" s="101"/>
+      <c r="B49" s="108"/>
+      <c r="C49" s="109"/>
+      <c r="D49" s="109"/>
+      <c r="E49" s="109"/>
+      <c r="F49" s="109"/>
+      <c r="G49" s="109"/>
+      <c r="H49" s="109"/>
+      <c r="I49" s="109"/>
+      <c r="J49" s="110"/>
     </row>
     <row r="50" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
-      <c r="C50" s="89" t="s">
+      <c r="C50" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="D50" s="90"/>
-      <c r="E50" s="90"/>
-      <c r="F50" s="90"/>
-      <c r="G50" s="90"/>
-      <c r="H50" s="90"/>
-      <c r="I50" s="90"/>
+      <c r="D50" s="106"/>
+      <c r="E50" s="106"/>
+      <c r="F50" s="106"/>
+      <c r="G50" s="106"/>
+      <c r="H50" s="106"/>
+      <c r="I50" s="106"/>
     </row>
     <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C51" s="61" t="s">
@@ -2355,7 +3063,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="91" t="s">
+      <c r="A52" s="98" t="s">
         <v>11</v>
       </c>
       <c r="B52" s="59" t="s">
@@ -2374,7 +3082,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="87"/>
+      <c r="A53" s="99"/>
       <c r="B53" s="2" t="s">
         <v>5</v>
       </c>
@@ -2391,7 +3099,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="87"/>
+      <c r="A54" s="99"/>
       <c r="B54" s="2" t="s">
         <v>6</v>
       </c>
@@ -2408,7 +3116,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="87"/>
+      <c r="A55" s="99"/>
       <c r="B55" s="2" t="s">
         <v>7</v>
       </c>
@@ -2425,7 +3133,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="87"/>
+      <c r="A56" s="99"/>
       <c r="B56" s="2" t="s">
         <v>8</v>
       </c>
@@ -2442,7 +3150,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="87"/>
+      <c r="A57" s="99"/>
       <c r="B57" s="2" t="s">
         <v>48</v>
       </c>
@@ -2459,7 +3167,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="87"/>
+      <c r="A58" s="99"/>
       <c r="B58" s="2" t="s">
         <v>9</v>
       </c>
@@ -2514,30 +3222,30 @@
       </c>
     </row>
     <row r="61" spans="1:10" s="52" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="102" t="s">
+      <c r="A61" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="B61" s="103"/>
-      <c r="C61" s="104"/>
-      <c r="D61" s="104"/>
-      <c r="E61" s="104"/>
-      <c r="F61" s="104"/>
-      <c r="G61" s="104"/>
-      <c r="H61" s="104"/>
-      <c r="I61" s="104"/>
-      <c r="J61" s="105"/>
+      <c r="B61" s="112"/>
+      <c r="C61" s="113"/>
+      <c r="D61" s="113"/>
+      <c r="E61" s="113"/>
+      <c r="F61" s="113"/>
+      <c r="G61" s="113"/>
+      <c r="H61" s="113"/>
+      <c r="I61" s="113"/>
+      <c r="J61" s="114"/>
     </row>
     <row r="62" spans="1:10" s="52" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
-      <c r="C62" s="89" t="s">
+      <c r="C62" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="D62" s="90"/>
-      <c r="E62" s="90"/>
-      <c r="F62" s="90"/>
-      <c r="G62" s="90"/>
-      <c r="H62" s="90"/>
-      <c r="I62" s="90"/>
+      <c r="D62" s="106"/>
+      <c r="E62" s="106"/>
+      <c r="F62" s="106"/>
+      <c r="G62" s="106"/>
+      <c r="H62" s="106"/>
+      <c r="I62" s="106"/>
       <c r="J62" s="51"/>
     </row>
     <row r="63" spans="1:10" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2567,7 +3275,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="91" t="s">
+      <c r="A64" s="98" t="s">
         <v>11</v>
       </c>
       <c r="B64" s="59" t="s">
@@ -2586,7 +3294,7 @@
       </c>
     </row>
     <row r="65" spans="1:10" s="52" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="87"/>
+      <c r="A65" s="99"/>
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
@@ -2603,7 +3311,7 @@
       </c>
     </row>
     <row r="66" spans="1:10" s="52" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="87"/>
+      <c r="A66" s="99"/>
       <c r="B66" s="2" t="s">
         <v>6</v>
       </c>
@@ -2620,7 +3328,7 @@
       </c>
     </row>
     <row r="67" spans="1:10" s="52" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="87"/>
+      <c r="A67" s="99"/>
       <c r="B67" s="2" t="s">
         <v>7</v>
       </c>
@@ -2637,7 +3345,7 @@
       </c>
     </row>
     <row r="68" spans="1:10" s="52" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="87"/>
+      <c r="A68" s="99"/>
       <c r="B68" s="2" t="s">
         <v>8</v>
       </c>
@@ -2654,7 +3362,7 @@
       </c>
     </row>
     <row r="69" spans="1:10" s="52" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="87"/>
+      <c r="A69" s="99"/>
       <c r="B69" s="2" t="s">
         <v>48</v>
       </c>
@@ -2671,7 +3379,7 @@
       </c>
     </row>
     <row r="70" spans="1:10" s="52" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="87"/>
+      <c r="A70" s="99"/>
       <c r="B70" s="2" t="s">
         <v>9</v>
       </c>
@@ -2736,30 +3444,30 @@
       <c r="J72" s="51"/>
     </row>
     <row r="73" spans="1:10" s="52" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="106" t="s">
+      <c r="A73" s="115" t="s">
         <v>60</v>
       </c>
-      <c r="B73" s="107"/>
-      <c r="C73" s="108"/>
-      <c r="D73" s="108"/>
-      <c r="E73" s="108"/>
-      <c r="F73" s="108"/>
-      <c r="G73" s="108"/>
-      <c r="H73" s="108"/>
-      <c r="I73" s="108"/>
-      <c r="J73" s="109"/>
+      <c r="B73" s="116"/>
+      <c r="C73" s="117"/>
+      <c r="D73" s="117"/>
+      <c r="E73" s="117"/>
+      <c r="F73" s="117"/>
+      <c r="G73" s="117"/>
+      <c r="H73" s="117"/>
+      <c r="I73" s="117"/>
+      <c r="J73" s="118"/>
     </row>
     <row r="74" spans="1:10" s="52" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="1"/>
-      <c r="C74" s="89" t="s">
+      <c r="C74" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="D74" s="90"/>
-      <c r="E74" s="90"/>
-      <c r="F74" s="90"/>
-      <c r="G74" s="90"/>
-      <c r="H74" s="90"/>
-      <c r="I74" s="90"/>
+      <c r="D74" s="106"/>
+      <c r="E74" s="106"/>
+      <c r="F74" s="106"/>
+      <c r="G74" s="106"/>
+      <c r="H74" s="106"/>
+      <c r="I74" s="106"/>
       <c r="J74" s="51"/>
     </row>
     <row r="75" spans="1:10" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2789,7 +3497,7 @@
       </c>
     </row>
     <row r="76" spans="1:10" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="91" t="s">
+      <c r="A76" s="98" t="s">
         <v>11</v>
       </c>
       <c r="B76" s="59" t="s">
@@ -2808,7 +3516,7 @@
       </c>
     </row>
     <row r="77" spans="1:10" s="52" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="87"/>
+      <c r="A77" s="99"/>
       <c r="B77" s="2" t="s">
         <v>5</v>
       </c>
@@ -2825,7 +3533,7 @@
       </c>
     </row>
     <row r="78" spans="1:10" s="52" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="87"/>
+      <c r="A78" s="99"/>
       <c r="B78" s="2" t="s">
         <v>6</v>
       </c>
@@ -2842,7 +3550,7 @@
       </c>
     </row>
     <row r="79" spans="1:10" s="52" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="87"/>
+      <c r="A79" s="99"/>
       <c r="B79" s="2" t="s">
         <v>7</v>
       </c>
@@ -2859,7 +3567,7 @@
       </c>
     </row>
     <row r="80" spans="1:10" s="52" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="87"/>
+      <c r="A80" s="99"/>
       <c r="B80" s="2" t="s">
         <v>8</v>
       </c>
@@ -2876,7 +3584,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" s="52" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="87"/>
+      <c r="A81" s="99"/>
       <c r="B81" s="2" t="s">
         <v>48</v>
       </c>
@@ -2893,7 +3601,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" s="52" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="87"/>
+      <c r="A82" s="99"/>
       <c r="B82" s="2" t="s">
         <v>9</v>
       </c>
@@ -2958,18 +3666,18 @@
       <c r="J84" s="51"/>
     </row>
     <row r="85" spans="1:10" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="85" t="s">
+      <c r="A85" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="B85" s="93"/>
-      <c r="C85" s="93"/>
-      <c r="D85" s="93"/>
-      <c r="E85" s="93"/>
-      <c r="F85" s="93"/>
-      <c r="G85" s="93"/>
-      <c r="H85" s="93"/>
-      <c r="I85" s="93"/>
-      <c r="J85" s="93"/>
+      <c r="B85" s="100"/>
+      <c r="C85" s="100"/>
+      <c r="D85" s="100"/>
+      <c r="E85" s="100"/>
+      <c r="F85" s="100"/>
+      <c r="G85" s="100"/>
+      <c r="H85" s="100"/>
+      <c r="I85" s="100"/>
+      <c r="J85" s="100"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="33" t="s">
@@ -2978,6 +3686,13 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A25:J25"/>
     <mergeCell ref="A52:A58"/>
     <mergeCell ref="A85:J85"/>
     <mergeCell ref="A28:A34"/>
@@ -2992,13 +3707,6 @@
     <mergeCell ref="A73:J73"/>
     <mergeCell ref="C74:I74"/>
     <mergeCell ref="A76:A82"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C14:I14"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="A25:J25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3028,18 +3736,18 @@
       <c r="A2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -3150,18 +3858,18 @@
       <c r="A12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="112" t="s">
+      <c r="A13" s="124" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="113"/>
-      <c r="C13" s="113"/>
-      <c r="D13" s="113"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="113"/>
-      <c r="G13" s="113"/>
-      <c r="H13" s="113"/>
-      <c r="I13" s="113"/>
-      <c r="J13" s="113"/>
+      <c r="B13" s="125"/>
+      <c r="C13" s="125"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="125"/>
+      <c r="F13" s="125"/>
+      <c r="G13" s="125"/>
+      <c r="H13" s="125"/>
+      <c r="I13" s="125"/>
+      <c r="J13" s="125"/>
     </row>
     <row r="14" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
@@ -3193,7 +3901,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="114"/>
+      <c r="A16" s="126"/>
       <c r="B16" s="59" t="s">
         <v>21</v>
       </c>
@@ -3219,7 +3927,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="87"/>
+      <c r="A17" s="99"/>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
@@ -3245,7 +3953,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="87"/>
+      <c r="A18" s="99"/>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
@@ -3271,7 +3979,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="87"/>
+      <c r="A19" s="99"/>
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
@@ -3297,7 +4005,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="87"/>
+      <c r="A20" s="99"/>
       <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
@@ -3323,7 +4031,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="87"/>
+      <c r="A21" s="99"/>
       <c r="B21" s="2" t="s">
         <v>48</v>
       </c>
@@ -3376,31 +4084,31 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="115" t="s">
+      <c r="A24" s="127" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="87"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="87"/>
+      <c r="B24" s="99"/>
+      <c r="C24" s="99"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
+      <c r="G24" s="99"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="99"/>
+      <c r="J24" s="99"/>
     </row>
     <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
-      <c r="C25" s="116" t="s">
+      <c r="C25" s="128" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="87"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
-      <c r="H25" s="87"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="87"/>
+      <c r="D25" s="99"/>
+      <c r="E25" s="99"/>
+      <c r="F25" s="99"/>
+      <c r="G25" s="99"/>
+      <c r="H25" s="99"/>
+      <c r="I25" s="99"/>
+      <c r="J25" s="99"/>
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C26" s="32" t="s">
@@ -3423,7 +4131,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="91" t="s">
+      <c r="A27" s="98" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="59" t="s">
@@ -3437,7 +4145,7 @@
       <c r="H27" s="48"/>
     </row>
     <row r="28" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="87"/>
+      <c r="A28" s="99"/>
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
@@ -3449,7 +4157,7 @@
       <c r="H28" s="48"/>
     </row>
     <row r="29" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="87"/>
+      <c r="A29" s="99"/>
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
@@ -3461,7 +4169,7 @@
       <c r="H29" s="48"/>
     </row>
     <row r="30" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="87"/>
+      <c r="A30" s="99"/>
       <c r="B30" s="2" t="s">
         <v>7</v>
       </c>
@@ -3473,7 +4181,7 @@
       <c r="H30" s="48"/>
     </row>
     <row r="31" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="87"/>
+      <c r="A31" s="99"/>
       <c r="B31" s="2" t="s">
         <v>8</v>
       </c>
@@ -3485,7 +4193,7 @@
       <c r="H31" s="48"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="87"/>
+      <c r="A32" s="99"/>
       <c r="B32" s="2" t="s">
         <v>48</v>
       </c>
@@ -3509,32 +4217,32 @@
       <c r="J33" s="36"/>
     </row>
     <row r="34" spans="1:10" s="38" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="110" t="s">
+      <c r="A34" s="122" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="111"/>
-      <c r="C34" s="111"/>
-      <c r="D34" s="111"/>
-      <c r="E34" s="111"/>
-      <c r="F34" s="111"/>
-      <c r="G34" s="111"/>
-      <c r="H34" s="111"/>
-      <c r="I34" s="111"/>
-      <c r="J34" s="111"/>
+      <c r="B34" s="123"/>
+      <c r="C34" s="123"/>
+      <c r="D34" s="123"/>
+      <c r="E34" s="123"/>
+      <c r="F34" s="123"/>
+      <c r="G34" s="123"/>
+      <c r="H34" s="123"/>
+      <c r="I34" s="123"/>
+      <c r="J34" s="123"/>
     </row>
     <row r="36" spans="1:10" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="85" t="s">
+      <c r="A36" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="93"/>
-      <c r="C36" s="93"/>
-      <c r="D36" s="93"/>
-      <c r="E36" s="93"/>
-      <c r="F36" s="93"/>
-      <c r="G36" s="93"/>
-      <c r="H36" s="93"/>
-      <c r="I36" s="93"/>
-      <c r="J36" s="93"/>
+      <c r="B36" s="100"/>
+      <c r="C36" s="100"/>
+      <c r="D36" s="100"/>
+      <c r="E36" s="100"/>
+      <c r="F36" s="100"/>
+      <c r="G36" s="100"/>
+      <c r="H36" s="100"/>
+      <c r="I36" s="100"/>
+      <c r="J36" s="100"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
@@ -3590,18 +4298,18 @@
       <c r="A2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="117"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="129"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -3695,18 +4403,18 @@
       <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="118" t="s">
+      <c r="A11" s="130" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="119"/>
-      <c r="C11" s="119"/>
-      <c r="D11" s="119"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="119"/>
-      <c r="G11" s="119"/>
-      <c r="H11" s="119"/>
-      <c r="I11" s="119"/>
-      <c r="J11" s="120"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="131"/>
+      <c r="D11" s="131"/>
+      <c r="E11" s="131"/>
+      <c r="F11" s="131"/>
+      <c r="G11" s="131"/>
+      <c r="H11" s="131"/>
+      <c r="I11" s="131"/>
+      <c r="J11" s="132"/>
     </row>
     <row r="12" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
@@ -3727,7 +4435,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="114"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="59" t="s">
         <v>21</v>
       </c>
@@ -3749,7 +4457,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="87"/>
+      <c r="A15" s="99"/>
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
@@ -3771,7 +4479,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="87"/>
+      <c r="A16" s="99"/>
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
@@ -3793,7 +4501,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="87"/>
+      <c r="A17" s="99"/>
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
@@ -3815,7 +4523,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="87"/>
+      <c r="A18" s="99"/>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -3837,7 +4545,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="87"/>
+      <c r="A19" s="99"/>
       <c r="B19" s="2" t="s">
         <v>48</v>
       </c>
@@ -3859,7 +4567,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="87"/>
+      <c r="A20" s="99"/>
       <c r="B20" s="2" t="s">
         <v>9</v>
       </c>
@@ -3906,30 +4614,30 @@
       <c r="D22" s="19"/>
     </row>
     <row r="23" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="121" t="s">
+      <c r="A23" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="87"/>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="117"/>
+      <c r="B23" s="99"/>
+      <c r="C23" s="99"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="99"/>
+      <c r="F23" s="99"/>
+      <c r="G23" s="99"/>
+      <c r="H23" s="99"/>
+      <c r="I23" s="99"/>
+      <c r="J23" s="129"/>
     </row>
     <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24" s="89" t="s">
+      <c r="C24" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
+      <c r="G24" s="99"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="99"/>
     </row>
     <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C25" s="60" t="s">
@@ -3958,7 +4666,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="91" t="s">
+      <c r="A26" s="98" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="59" t="s">
@@ -3977,7 +4685,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="87"/>
+      <c r="A27" s="99"/>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
@@ -3994,7 +4702,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="87"/>
+      <c r="A28" s="99"/>
       <c r="B28" s="2" t="s">
         <v>6</v>
       </c>
@@ -4011,7 +4719,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="87"/>
+      <c r="A29" s="99"/>
       <c r="B29" s="2" t="s">
         <v>7</v>
       </c>
@@ -4028,7 +4736,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="87"/>
+      <c r="A30" s="99"/>
       <c r="B30" s="2" t="s">
         <v>8</v>
       </c>
@@ -4045,7 +4753,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="87"/>
+      <c r="A31" s="99"/>
       <c r="B31" s="2" t="s">
         <v>48</v>
       </c>
@@ -4062,7 +4770,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="87"/>
+      <c r="A32" s="99"/>
       <c r="B32" s="2" t="s">
         <v>9</v>
       </c>
@@ -4117,18 +4825,18 @@
       </c>
     </row>
     <row r="35" spans="1:10" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="85" t="s">
+      <c r="A35" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="93"/>
-      <c r="C35" s="93"/>
-      <c r="D35" s="93"/>
-      <c r="E35" s="93"/>
-      <c r="F35" s="93"/>
-      <c r="G35" s="93"/>
-      <c r="H35" s="93"/>
-      <c r="I35" s="93"/>
-      <c r="J35" s="93"/>
+      <c r="B35" s="100"/>
+      <c r="C35" s="100"/>
+      <c r="D35" s="100"/>
+      <c r="E35" s="100"/>
+      <c r="F35" s="100"/>
+      <c r="G35" s="100"/>
+      <c r="H35" s="100"/>
+      <c r="I35" s="100"/>
+      <c r="J35" s="100"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="33" t="s">
@@ -4200,18 +4908,18 @@
       <c r="J2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="117"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="129"/>
     </row>
     <row r="4" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="66"/>
@@ -4220,10 +4928,10 @@
       <c r="D4" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="132" t="s">
+      <c r="E4" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="133" t="s">
+      <c r="F4" s="95" t="s">
         <v>65</v>
       </c>
       <c r="G4" s="63" t="s">
@@ -4242,11 +4950,11 @@
         <f>'SDG 15.3.1'!F5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="122" t="e">
+      <c r="E5" s="84" t="e">
         <f>'SDG 15.3.1'!G5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F5" s="123">
+      <c r="F5" s="85">
         <f>SUM(F6:F9)</f>
         <v>0</v>
       </c>
@@ -4267,11 +4975,11 @@
         <f>'SDG 15.3.1'!F6</f>
         <v>0</v>
       </c>
-      <c r="E6" s="124" t="e">
+      <c r="E6" s="86" t="e">
         <f>'SDG 15.3.1'!G6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F6" s="125"/>
+      <c r="F6" s="87"/>
       <c r="G6" s="80" t="e">
         <f>F6/F$5</f>
         <v>#DIV/0!</v>
@@ -4289,11 +4997,11 @@
         <f>'SDG 15.3.1'!F8</f>
         <v>0</v>
       </c>
-      <c r="E7" s="126" t="e">
+      <c r="E7" s="88" t="e">
         <f>'SDG 15.3.1'!G7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F7" s="127"/>
+      <c r="F7" s="89"/>
       <c r="G7" s="81" t="e">
         <f>F7/F$5</f>
         <v>#DIV/0!</v>
@@ -4311,11 +5019,11 @@
         <f>'SDG 15.3.1'!F8</f>
         <v>0</v>
       </c>
-      <c r="E8" s="128" t="e">
+      <c r="E8" s="90" t="e">
         <f>'SDG 15.3.1'!G8</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F8" s="129"/>
+      <c r="F8" s="91"/>
       <c r="G8" s="82" t="e">
         <f>F8/F$5</f>
         <v>#DIV/0!</v>
@@ -4333,11 +5041,11 @@
         <f>'SDG 15.3.1'!F9</f>
         <v>0</v>
       </c>
-      <c r="E9" s="130" t="e">
+      <c r="E9" s="92" t="e">
         <f>'SDG 15.3.1'!G9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F9" s="131"/>
+      <c r="F9" s="93"/>
       <c r="G9" s="83" t="e">
         <f>F9/F$5</f>
         <v>#DIV/0!</v>
@@ -4370,18 +5078,18 @@
       <c r="J11" s="65"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="85" t="s">
+      <c r="A12" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="93"/>
-      <c r="C12" s="93"/>
-      <c r="D12" s="93"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="93"/>
-      <c r="G12" s="93"/>
-      <c r="H12" s="93"/>
-      <c r="I12" s="93"/>
-      <c r="J12" s="93"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="100"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="100"/>
+      <c r="F12" s="100"/>
+      <c r="G12" s="100"/>
+      <c r="H12" s="100"/>
+      <c r="I12" s="100"/>
+      <c r="J12" s="100"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="64"/>
@@ -4417,4 +5125,1557 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84595693-2766-4438-88C6-66C4A1683268}">
+  <dimension ref="A1:Z107"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="134" customWidth="1"/>
+    <col min="2" max="10" width="20.7109375" style="134" customWidth="1"/>
+    <col min="11" max="16384" width="14.42578125" style="134"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="96" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="129"/>
+    </row>
+    <row r="4" spans="1:26" s="152" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="150"/>
+      <c r="B4" s="151"/>
+      <c r="C4" s="151"/>
+      <c r="D4" s="151"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="151"/>
+      <c r="G4" s="151"/>
+      <c r="H4" s="151"/>
+      <c r="I4" s="151"/>
+      <c r="J4" s="151"/>
+      <c r="K4" s="151"/>
+      <c r="L4" s="151"/>
+      <c r="M4" s="151"/>
+      <c r="N4" s="151"/>
+      <c r="O4" s="151"/>
+      <c r="P4" s="151"/>
+      <c r="Q4" s="151"/>
+      <c r="R4" s="151"/>
+      <c r="S4" s="151"/>
+      <c r="T4" s="151"/>
+      <c r="U4" s="151"/>
+      <c r="V4" s="151"/>
+      <c r="W4" s="151"/>
+      <c r="X4" s="151"/>
+      <c r="Y4" s="151"/>
+      <c r="Z4" s="151"/>
+    </row>
+    <row r="5" spans="1:26" s="154" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="71" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="135" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="138" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="138" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="138" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="138" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="138" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="138" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="139" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" s="138" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="141"/>
+      <c r="B7" s="141"/>
+      <c r="C7" s="142"/>
+      <c r="D7" s="142"/>
+      <c r="E7" s="142"/>
+      <c r="F7" s="142"/>
+      <c r="G7" s="142"/>
+      <c r="H7" s="143"/>
+      <c r="I7" s="142"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="141"/>
+      <c r="B8" s="141"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="142"/>
+      <c r="F8" s="142"/>
+      <c r="G8" s="142"/>
+      <c r="H8" s="143"/>
+      <c r="I8" s="142"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="141"/>
+      <c r="B9" s="141"/>
+      <c r="C9" s="142"/>
+      <c r="D9" s="142"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="142"/>
+      <c r="G9" s="142"/>
+      <c r="H9" s="143"/>
+      <c r="I9" s="142"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="141"/>
+      <c r="B10" s="141"/>
+      <c r="C10" s="142"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="142"/>
+      <c r="F10" s="142"/>
+      <c r="G10" s="142"/>
+      <c r="H10" s="143"/>
+      <c r="I10" s="142"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="141"/>
+      <c r="B11" s="141"/>
+      <c r="C11" s="142"/>
+      <c r="D11" s="142"/>
+      <c r="E11" s="142"/>
+      <c r="F11" s="142"/>
+      <c r="G11" s="142"/>
+      <c r="H11" s="143"/>
+      <c r="I11" s="142"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="141"/>
+      <c r="B12" s="141"/>
+      <c r="C12" s="142"/>
+      <c r="D12" s="142"/>
+      <c r="E12" s="142"/>
+      <c r="F12" s="142"/>
+      <c r="G12" s="142"/>
+      <c r="H12" s="143"/>
+      <c r="I12" s="142"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="141"/>
+      <c r="B13" s="141"/>
+      <c r="C13" s="142"/>
+      <c r="D13" s="142"/>
+      <c r="E13" s="142"/>
+      <c r="F13" s="142"/>
+      <c r="G13" s="142"/>
+      <c r="H13" s="143"/>
+      <c r="I13" s="142"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="141"/>
+      <c r="B14" s="141"/>
+      <c r="C14" s="142"/>
+      <c r="D14" s="142"/>
+      <c r="E14" s="142"/>
+      <c r="F14" s="142"/>
+      <c r="G14" s="142"/>
+      <c r="H14" s="143"/>
+      <c r="I14" s="142"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="141"/>
+      <c r="B15" s="141"/>
+      <c r="C15" s="142"/>
+      <c r="D15" s="142"/>
+      <c r="E15" s="142"/>
+      <c r="F15" s="142"/>
+      <c r="G15" s="142"/>
+      <c r="H15" s="143"/>
+      <c r="I15" s="142"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="141"/>
+      <c r="B16" s="141"/>
+      <c r="C16" s="142"/>
+      <c r="D16" s="142"/>
+      <c r="E16" s="142"/>
+      <c r="F16" s="142"/>
+      <c r="G16" s="142"/>
+      <c r="H16" s="143"/>
+      <c r="I16" s="142"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="141"/>
+      <c r="B17" s="141"/>
+      <c r="C17" s="142"/>
+      <c r="D17" s="142"/>
+      <c r="E17" s="142"/>
+      <c r="F17" s="142"/>
+      <c r="G17" s="142"/>
+      <c r="H17" s="143"/>
+      <c r="I17" s="142"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="141"/>
+      <c r="B18" s="141"/>
+      <c r="C18" s="142"/>
+      <c r="D18" s="142"/>
+      <c r="E18" s="142"/>
+      <c r="F18" s="142"/>
+      <c r="G18" s="142"/>
+      <c r="H18" s="143"/>
+      <c r="I18" s="142"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="141"/>
+      <c r="B19" s="141"/>
+      <c r="C19" s="142"/>
+      <c r="D19" s="142"/>
+      <c r="E19" s="142"/>
+      <c r="F19" s="142"/>
+      <c r="G19" s="142"/>
+      <c r="H19" s="143"/>
+      <c r="I19" s="142"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="141"/>
+      <c r="B20" s="141"/>
+      <c r="C20" s="142"/>
+      <c r="D20" s="142"/>
+      <c r="E20" s="142"/>
+      <c r="F20" s="142"/>
+      <c r="G20" s="142"/>
+      <c r="H20" s="143"/>
+      <c r="I20" s="142"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="141"/>
+      <c r="B21" s="141"/>
+      <c r="C21" s="142"/>
+      <c r="D21" s="142"/>
+      <c r="E21" s="142"/>
+      <c r="F21" s="142"/>
+      <c r="G21" s="142"/>
+      <c r="H21" s="143"/>
+      <c r="I21" s="142"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="141"/>
+      <c r="B22" s="141"/>
+      <c r="C22" s="142"/>
+      <c r="D22" s="142"/>
+      <c r="E22" s="142"/>
+      <c r="F22" s="142"/>
+      <c r="G22" s="142"/>
+      <c r="H22" s="143"/>
+      <c r="I22" s="142"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="141"/>
+      <c r="B23" s="141"/>
+      <c r="C23" s="142"/>
+      <c r="D23" s="142"/>
+      <c r="E23" s="142"/>
+      <c r="F23" s="142"/>
+      <c r="G23" s="142"/>
+      <c r="H23" s="143"/>
+      <c r="I23" s="142"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="141"/>
+      <c r="B24" s="141"/>
+      <c r="C24" s="142"/>
+      <c r="D24" s="142"/>
+      <c r="E24" s="142"/>
+      <c r="F24" s="142"/>
+      <c r="G24" s="142"/>
+      <c r="H24" s="143"/>
+      <c r="I24" s="142"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="141"/>
+      <c r="B25" s="141"/>
+      <c r="C25" s="142"/>
+      <c r="D25" s="142"/>
+      <c r="E25" s="142"/>
+      <c r="F25" s="142"/>
+      <c r="G25" s="142"/>
+      <c r="H25" s="143"/>
+      <c r="I25" s="142"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="141"/>
+      <c r="B26" s="141"/>
+      <c r="C26" s="142"/>
+      <c r="D26" s="142"/>
+      <c r="E26" s="142"/>
+      <c r="F26" s="142"/>
+      <c r="G26" s="142"/>
+      <c r="H26" s="143"/>
+      <c r="I26" s="142"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="141"/>
+      <c r="B27" s="141"/>
+      <c r="C27" s="142"/>
+      <c r="D27" s="142"/>
+      <c r="E27" s="142"/>
+      <c r="F27" s="142"/>
+      <c r="G27" s="142"/>
+      <c r="H27" s="143"/>
+      <c r="I27" s="142"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="141"/>
+      <c r="B28" s="141"/>
+      <c r="C28" s="142"/>
+      <c r="D28" s="142"/>
+      <c r="E28" s="142"/>
+      <c r="F28" s="142"/>
+      <c r="G28" s="142"/>
+      <c r="H28" s="143"/>
+      <c r="I28" s="142"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="141"/>
+      <c r="B29" s="141"/>
+      <c r="C29" s="142"/>
+      <c r="D29" s="142"/>
+      <c r="E29" s="142"/>
+      <c r="F29" s="142"/>
+      <c r="G29" s="142"/>
+      <c r="H29" s="143"/>
+      <c r="I29" s="142"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="141"/>
+      <c r="B30" s="141"/>
+      <c r="C30" s="142"/>
+      <c r="D30" s="142"/>
+      <c r="E30" s="142"/>
+      <c r="F30" s="142"/>
+      <c r="G30" s="142"/>
+      <c r="H30" s="143"/>
+      <c r="I30" s="142"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="141"/>
+      <c r="B31" s="141"/>
+      <c r="C31" s="142"/>
+      <c r="D31" s="142"/>
+      <c r="E31" s="142"/>
+      <c r="F31" s="142"/>
+      <c r="G31" s="142"/>
+      <c r="H31" s="143"/>
+      <c r="I31" s="142"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="141"/>
+      <c r="B32" s="141"/>
+      <c r="C32" s="142"/>
+      <c r="D32" s="142"/>
+      <c r="E32" s="142"/>
+      <c r="F32" s="142"/>
+      <c r="G32" s="142"/>
+      <c r="H32" s="143"/>
+      <c r="I32" s="142"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="141"/>
+      <c r="B33" s="141"/>
+      <c r="C33" s="142"/>
+      <c r="D33" s="142"/>
+      <c r="E33" s="142"/>
+      <c r="F33" s="142"/>
+      <c r="G33" s="142"/>
+      <c r="H33" s="143"/>
+      <c r="I33" s="142"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="141"/>
+      <c r="B34" s="141"/>
+      <c r="C34" s="142"/>
+      <c r="D34" s="142"/>
+      <c r="E34" s="142"/>
+      <c r="F34" s="142"/>
+      <c r="G34" s="142"/>
+      <c r="H34" s="143"/>
+      <c r="I34" s="142"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="141"/>
+      <c r="B35" s="141"/>
+      <c r="C35" s="142"/>
+      <c r="D35" s="142"/>
+      <c r="E35" s="142"/>
+      <c r="F35" s="142"/>
+      <c r="G35" s="142"/>
+      <c r="H35" s="143"/>
+      <c r="I35" s="142"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="141"/>
+      <c r="B36" s="141"/>
+      <c r="C36" s="142"/>
+      <c r="D36" s="142"/>
+      <c r="E36" s="142"/>
+      <c r="F36" s="142"/>
+      <c r="G36" s="142"/>
+      <c r="H36" s="143"/>
+      <c r="I36" s="142"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="155"/>
+      <c r="B37" s="155"/>
+      <c r="C37" s="156"/>
+      <c r="D37" s="156"/>
+      <c r="E37" s="156"/>
+      <c r="F37" s="156"/>
+      <c r="G37" s="156"/>
+      <c r="H37" s="156"/>
+      <c r="I37" s="156"/>
+    </row>
+    <row r="38" spans="1:9" s="154" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="71" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="135" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="138" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="138" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="138" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="138" t="s">
+        <v>91</v>
+      </c>
+      <c r="F39" s="138" t="s">
+        <v>96</v>
+      </c>
+      <c r="G39" s="138" t="s">
+        <v>92</v>
+      </c>
+      <c r="H39" s="139" t="s">
+        <v>93</v>
+      </c>
+      <c r="I39" s="138" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="141"/>
+      <c r="B40" s="141"/>
+      <c r="C40" s="142"/>
+      <c r="D40" s="142"/>
+      <c r="E40" s="142"/>
+      <c r="F40" s="142"/>
+      <c r="G40" s="142"/>
+      <c r="H40" s="143"/>
+      <c r="I40" s="142"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="141"/>
+      <c r="B41" s="141"/>
+      <c r="C41" s="142"/>
+      <c r="D41" s="142"/>
+      <c r="E41" s="142"/>
+      <c r="F41" s="142"/>
+      <c r="G41" s="142"/>
+      <c r="H41" s="143"/>
+      <c r="I41" s="142"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="141"/>
+      <c r="B42" s="141"/>
+      <c r="C42" s="142"/>
+      <c r="D42" s="142"/>
+      <c r="E42" s="142"/>
+      <c r="F42" s="142"/>
+      <c r="G42" s="142"/>
+      <c r="H42" s="143"/>
+      <c r="I42" s="142"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="141"/>
+      <c r="B43" s="141"/>
+      <c r="C43" s="142"/>
+      <c r="D43" s="142"/>
+      <c r="E43" s="142"/>
+      <c r="F43" s="142"/>
+      <c r="G43" s="142"/>
+      <c r="H43" s="143"/>
+      <c r="I43" s="142"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="141"/>
+      <c r="B44" s="141"/>
+      <c r="C44" s="142"/>
+      <c r="D44" s="142"/>
+      <c r="E44" s="142"/>
+      <c r="F44" s="142"/>
+      <c r="G44" s="142"/>
+      <c r="H44" s="143"/>
+      <c r="I44" s="142"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="141"/>
+      <c r="B45" s="141"/>
+      <c r="C45" s="142"/>
+      <c r="D45" s="142"/>
+      <c r="E45" s="142"/>
+      <c r="F45" s="142"/>
+      <c r="G45" s="142"/>
+      <c r="H45" s="143"/>
+      <c r="I45" s="142"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="141"/>
+      <c r="B46" s="141"/>
+      <c r="C46" s="142"/>
+      <c r="D46" s="142"/>
+      <c r="E46" s="142"/>
+      <c r="F46" s="142"/>
+      <c r="G46" s="142"/>
+      <c r="H46" s="143"/>
+      <c r="I46" s="142"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="141"/>
+      <c r="B47" s="141"/>
+      <c r="C47" s="142"/>
+      <c r="D47" s="142"/>
+      <c r="E47" s="142"/>
+      <c r="F47" s="142"/>
+      <c r="G47" s="142"/>
+      <c r="H47" s="143"/>
+      <c r="I47" s="142"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="141"/>
+      <c r="B48" s="141"/>
+      <c r="C48" s="142"/>
+      <c r="D48" s="142"/>
+      <c r="E48" s="142"/>
+      <c r="F48" s="142"/>
+      <c r="G48" s="142"/>
+      <c r="H48" s="143"/>
+      <c r="I48" s="142"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="141"/>
+      <c r="B49" s="141"/>
+      <c r="C49" s="142"/>
+      <c r="D49" s="142"/>
+      <c r="E49" s="142"/>
+      <c r="F49" s="142"/>
+      <c r="G49" s="142"/>
+      <c r="H49" s="143"/>
+      <c r="I49" s="142"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="141"/>
+      <c r="B50" s="141"/>
+      <c r="C50" s="142"/>
+      <c r="D50" s="142"/>
+      <c r="E50" s="142"/>
+      <c r="F50" s="142"/>
+      <c r="G50" s="142"/>
+      <c r="H50" s="143"/>
+      <c r="I50" s="142"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="141"/>
+      <c r="B51" s="141"/>
+      <c r="C51" s="142"/>
+      <c r="D51" s="142"/>
+      <c r="E51" s="142"/>
+      <c r="F51" s="142"/>
+      <c r="G51" s="142"/>
+      <c r="H51" s="143"/>
+      <c r="I51" s="142"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="141"/>
+      <c r="B52" s="141"/>
+      <c r="C52" s="142"/>
+      <c r="D52" s="142"/>
+      <c r="E52" s="142"/>
+      <c r="F52" s="142"/>
+      <c r="G52" s="142"/>
+      <c r="H52" s="143"/>
+      <c r="I52" s="142"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="141"/>
+      <c r="B53" s="141"/>
+      <c r="C53" s="142"/>
+      <c r="D53" s="142"/>
+      <c r="E53" s="142"/>
+      <c r="F53" s="142"/>
+      <c r="G53" s="142"/>
+      <c r="H53" s="143"/>
+      <c r="I53" s="142"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="141"/>
+      <c r="B54" s="141"/>
+      <c r="C54" s="142"/>
+      <c r="D54" s="142"/>
+      <c r="E54" s="142"/>
+      <c r="F54" s="142"/>
+      <c r="G54" s="142"/>
+      <c r="H54" s="143"/>
+      <c r="I54" s="142"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="141"/>
+      <c r="B55" s="141"/>
+      <c r="C55" s="142"/>
+      <c r="D55" s="142"/>
+      <c r="E55" s="142"/>
+      <c r="F55" s="142"/>
+      <c r="G55" s="142"/>
+      <c r="H55" s="143"/>
+      <c r="I55" s="142"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="141"/>
+      <c r="B56" s="141"/>
+      <c r="C56" s="142"/>
+      <c r="D56" s="142"/>
+      <c r="E56" s="142"/>
+      <c r="F56" s="142"/>
+      <c r="G56" s="142"/>
+      <c r="H56" s="143"/>
+      <c r="I56" s="142"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="141"/>
+      <c r="B57" s="141"/>
+      <c r="C57" s="142"/>
+      <c r="D57" s="142"/>
+      <c r="E57" s="142"/>
+      <c r="F57" s="142"/>
+      <c r="G57" s="142"/>
+      <c r="H57" s="143"/>
+      <c r="I57" s="142"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="141"/>
+      <c r="B58" s="141"/>
+      <c r="C58" s="142"/>
+      <c r="D58" s="142"/>
+      <c r="E58" s="142"/>
+      <c r="F58" s="142"/>
+      <c r="G58" s="142"/>
+      <c r="H58" s="143"/>
+      <c r="I58" s="142"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="141"/>
+      <c r="B59" s="141"/>
+      <c r="C59" s="142"/>
+      <c r="D59" s="142"/>
+      <c r="E59" s="142"/>
+      <c r="F59" s="142"/>
+      <c r="G59" s="142"/>
+      <c r="H59" s="143"/>
+      <c r="I59" s="142"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="141"/>
+      <c r="B60" s="141"/>
+      <c r="C60" s="142"/>
+      <c r="D60" s="142"/>
+      <c r="E60" s="142"/>
+      <c r="F60" s="142"/>
+      <c r="G60" s="142"/>
+      <c r="H60" s="143"/>
+      <c r="I60" s="142"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="141"/>
+      <c r="B61" s="141"/>
+      <c r="C61" s="142"/>
+      <c r="D61" s="142"/>
+      <c r="E61" s="142"/>
+      <c r="F61" s="142"/>
+      <c r="G61" s="142"/>
+      <c r="H61" s="143"/>
+      <c r="I61" s="142"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="141"/>
+      <c r="B62" s="141"/>
+      <c r="C62" s="142"/>
+      <c r="D62" s="142"/>
+      <c r="E62" s="142"/>
+      <c r="F62" s="142"/>
+      <c r="G62" s="142"/>
+      <c r="H62" s="143"/>
+      <c r="I62" s="142"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="141"/>
+      <c r="B63" s="141"/>
+      <c r="C63" s="142"/>
+      <c r="D63" s="142"/>
+      <c r="E63" s="142"/>
+      <c r="F63" s="142"/>
+      <c r="G63" s="142"/>
+      <c r="H63" s="143"/>
+      <c r="I63" s="142"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="141"/>
+      <c r="B64" s="141"/>
+      <c r="C64" s="142"/>
+      <c r="D64" s="142"/>
+      <c r="E64" s="142"/>
+      <c r="F64" s="142"/>
+      <c r="G64" s="142"/>
+      <c r="H64" s="143"/>
+      <c r="I64" s="142"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="141"/>
+      <c r="B65" s="141"/>
+      <c r="C65" s="142"/>
+      <c r="D65" s="142"/>
+      <c r="E65" s="142"/>
+      <c r="F65" s="142"/>
+      <c r="G65" s="142"/>
+      <c r="H65" s="143"/>
+      <c r="I65" s="142"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="141"/>
+      <c r="B66" s="141"/>
+      <c r="C66" s="142"/>
+      <c r="D66" s="142"/>
+      <c r="E66" s="142"/>
+      <c r="F66" s="142"/>
+      <c r="G66" s="142"/>
+      <c r="H66" s="143"/>
+      <c r="I66" s="142"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="141"/>
+      <c r="B67" s="141"/>
+      <c r="C67" s="142"/>
+      <c r="D67" s="142"/>
+      <c r="E67" s="142"/>
+      <c r="F67" s="142"/>
+      <c r="G67" s="142"/>
+      <c r="H67" s="143"/>
+      <c r="I67" s="142"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="141"/>
+      <c r="B68" s="141"/>
+      <c r="C68" s="142"/>
+      <c r="D68" s="142"/>
+      <c r="E68" s="142"/>
+      <c r="F68" s="142"/>
+      <c r="G68" s="142"/>
+      <c r="H68" s="143"/>
+      <c r="I68" s="142"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="141"/>
+      <c r="B69" s="141"/>
+      <c r="C69" s="142"/>
+      <c r="D69" s="142"/>
+      <c r="E69" s="142"/>
+      <c r="F69" s="142"/>
+      <c r="G69" s="142"/>
+      <c r="H69" s="143"/>
+      <c r="I69" s="142"/>
+    </row>
+    <row r="70" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:10" s="154" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="71" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B72" s="141"/>
+      <c r="C72" s="138" t="s">
+        <v>21</v>
+      </c>
+      <c r="D72" s="138" t="s">
+        <v>5</v>
+      </c>
+      <c r="E72" s="138" t="s">
+        <v>6</v>
+      </c>
+      <c r="F72" s="138" t="s">
+        <v>7</v>
+      </c>
+      <c r="G72" s="138" t="s">
+        <v>72</v>
+      </c>
+      <c r="H72" s="138" t="s">
+        <v>73</v>
+      </c>
+      <c r="I72" s="138" t="s">
+        <v>9</v>
+      </c>
+      <c r="J72" s="138" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="138" t="s">
+        <v>21</v>
+      </c>
+      <c r="C73" s="142"/>
+      <c r="D73" s="142"/>
+      <c r="E73" s="142"/>
+      <c r="F73" s="142"/>
+      <c r="G73" s="142"/>
+      <c r="H73" s="142"/>
+      <c r="I73" s="142"/>
+      <c r="J73" s="141">
+        <f t="shared" ref="J73:J80" si="0">SUM(C73:I73)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="138" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="142"/>
+      <c r="D74" s="142"/>
+      <c r="E74" s="142"/>
+      <c r="F74" s="142"/>
+      <c r="G74" s="142"/>
+      <c r="H74" s="142"/>
+      <c r="I74" s="142"/>
+      <c r="J74" s="141">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="138" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" s="142"/>
+      <c r="D75" s="142"/>
+      <c r="E75" s="142"/>
+      <c r="F75" s="142"/>
+      <c r="G75" s="142"/>
+      <c r="H75" s="142"/>
+      <c r="I75" s="142"/>
+      <c r="J75" s="141">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="138" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="142"/>
+      <c r="D76" s="142"/>
+      <c r="E76" s="142"/>
+      <c r="F76" s="142"/>
+      <c r="G76" s="142"/>
+      <c r="H76" s="142"/>
+      <c r="I76" s="142"/>
+      <c r="J76" s="141">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="138" t="s">
+        <v>72</v>
+      </c>
+      <c r="C77" s="142"/>
+      <c r="D77" s="142"/>
+      <c r="E77" s="142"/>
+      <c r="F77" s="142"/>
+      <c r="G77" s="142"/>
+      <c r="H77" s="142"/>
+      <c r="I77" s="142"/>
+      <c r="J77" s="141">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="138" t="s">
+        <v>73</v>
+      </c>
+      <c r="C78" s="142"/>
+      <c r="D78" s="142"/>
+      <c r="E78" s="142"/>
+      <c r="F78" s="142"/>
+      <c r="G78" s="142"/>
+      <c r="H78" s="142"/>
+      <c r="I78" s="142"/>
+      <c r="J78" s="141">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="138" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" s="142"/>
+      <c r="D79" s="142"/>
+      <c r="E79" s="142"/>
+      <c r="F79" s="142"/>
+      <c r="G79" s="142"/>
+      <c r="H79" s="142"/>
+      <c r="I79" s="142"/>
+      <c r="J79" s="141">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="138" t="s">
+        <v>80</v>
+      </c>
+      <c r="C80" s="142">
+        <f t="shared" ref="C80:I80" si="1">SUM(C73:C79)</f>
+        <v>0</v>
+      </c>
+      <c r="D80" s="142">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E80" s="142">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F80" s="142">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G80" s="142">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H80" s="142">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I80" s="142">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J80" s="141">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:10" s="154" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="71" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B83" s="141"/>
+      <c r="C83" s="138" t="s">
+        <v>21</v>
+      </c>
+      <c r="D83" s="138" t="s">
+        <v>5</v>
+      </c>
+      <c r="E83" s="138" t="s">
+        <v>6</v>
+      </c>
+      <c r="F83" s="138" t="s">
+        <v>7</v>
+      </c>
+      <c r="G83" s="138" t="s">
+        <v>72</v>
+      </c>
+      <c r="H83" s="138" t="s">
+        <v>73</v>
+      </c>
+      <c r="I83" s="138" t="s">
+        <v>9</v>
+      </c>
+      <c r="J83" s="138" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="138" t="s">
+        <v>21</v>
+      </c>
+      <c r="C84" s="142"/>
+      <c r="D84" s="142"/>
+      <c r="E84" s="142"/>
+      <c r="F84" s="142"/>
+      <c r="G84" s="142"/>
+      <c r="H84" s="142"/>
+      <c r="I84" s="142"/>
+      <c r="J84" s="141">
+        <f t="shared" ref="J84:J91" si="2">SUM(C84:I84)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="138" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" s="142"/>
+      <c r="D85" s="142"/>
+      <c r="E85" s="142"/>
+      <c r="F85" s="142"/>
+      <c r="G85" s="142"/>
+      <c r="H85" s="142"/>
+      <c r="I85" s="142"/>
+      <c r="J85" s="141">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="138" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" s="142"/>
+      <c r="D86" s="142"/>
+      <c r="E86" s="142"/>
+      <c r="F86" s="142"/>
+      <c r="G86" s="142"/>
+      <c r="H86" s="142"/>
+      <c r="I86" s="142"/>
+      <c r="J86" s="141">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="138" t="s">
+        <v>7</v>
+      </c>
+      <c r="C87" s="142"/>
+      <c r="D87" s="142"/>
+      <c r="E87" s="142"/>
+      <c r="F87" s="142"/>
+      <c r="G87" s="142"/>
+      <c r="H87" s="142"/>
+      <c r="I87" s="142"/>
+      <c r="J87" s="141">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="138" t="s">
+        <v>72</v>
+      </c>
+      <c r="C88" s="142"/>
+      <c r="D88" s="142"/>
+      <c r="E88" s="142"/>
+      <c r="F88" s="142"/>
+      <c r="G88" s="142"/>
+      <c r="H88" s="142"/>
+      <c r="I88" s="142"/>
+      <c r="J88" s="141">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="138" t="s">
+        <v>73</v>
+      </c>
+      <c r="C89" s="142"/>
+      <c r="D89" s="142"/>
+      <c r="E89" s="142"/>
+      <c r="F89" s="142"/>
+      <c r="G89" s="142"/>
+      <c r="H89" s="142"/>
+      <c r="I89" s="142"/>
+      <c r="J89" s="141">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="138" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" s="142"/>
+      <c r="D90" s="142"/>
+      <c r="E90" s="142"/>
+      <c r="F90" s="142"/>
+      <c r="G90" s="142"/>
+      <c r="H90" s="142"/>
+      <c r="I90" s="142"/>
+      <c r="J90" s="141">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="138" t="s">
+        <v>80</v>
+      </c>
+      <c r="C91" s="142">
+        <f t="shared" ref="C91:I91" si="3">SUM(C84:C90)</f>
+        <v>0</v>
+      </c>
+      <c r="D91" s="142">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E91" s="142">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F91" s="142">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G91" s="142">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H91" s="142">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I91" s="142">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J91" s="141">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="137"/>
+    </row>
+    <row r="93" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="1:10" s="154" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="154" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="145"/>
+      <c r="B95" s="135" t="s">
+        <v>84</v>
+      </c>
+      <c r="C95" s="135" t="s">
+        <v>74</v>
+      </c>
+      <c r="D95" s="146"/>
+    </row>
+    <row r="96" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="135" t="s">
+        <v>75</v>
+      </c>
+      <c r="B96" s="147"/>
+      <c r="C96" s="148" t="str">
+        <f>IFERROR((B96/#REF!)*100,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="D96" s="149"/>
+    </row>
+    <row r="97" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="135" t="s">
+        <v>79</v>
+      </c>
+      <c r="B97" s="147"/>
+      <c r="C97" s="148" t="str">
+        <f>IFERROR((B97/#REF!)*100,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="D97" s="149"/>
+    </row>
+    <row r="98" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="135" t="s">
+        <v>76</v>
+      </c>
+      <c r="B98" s="147"/>
+      <c r="C98" s="148" t="str">
+        <f>IFERROR((B98/#REF!)*100,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="D98" s="149"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="136"/>
+    </row>
+    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="1:4" s="154" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="154" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="138"/>
+      <c r="B102" s="157" t="s">
+        <v>84</v>
+      </c>
+      <c r="C102" s="158" t="s">
+        <v>74</v>
+      </c>
+      <c r="D102" s="140"/>
+    </row>
+    <row r="103" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="138" t="s">
+        <v>78</v>
+      </c>
+      <c r="B103" s="159"/>
+      <c r="C103" s="160" t="str">
+        <f>IFERROR((B103/#REF!)*100,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="D103" s="144"/>
+    </row>
+    <row r="104" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="138" t="s">
+        <v>77</v>
+      </c>
+      <c r="B104" s="159"/>
+      <c r="C104" s="160" t="str">
+        <f>IFERROR((B104/#REF!)*100,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="D104" s="144"/>
+    </row>
+    <row r="105" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="138" t="s">
+        <v>75</v>
+      </c>
+      <c r="B105" s="159"/>
+      <c r="C105" s="160" t="str">
+        <f>IFERROR((B105/#REF!)*100,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="D105" s="144"/>
+    </row>
+    <row r="106" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="153" t="s">
+        <v>76</v>
+      </c>
+      <c r="B106" s="161"/>
+      <c r="C106" s="160" t="str">
+        <f>IFERROR((B106/#REF!)*100,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="D106" s="144"/>
+    </row>
+    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:J3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A107:Z107 A117:Z987">
+    <cfRule type="expression" dxfId="53" priority="33">
+      <formula>_xludf.isformula(A107:Z1127)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A102:Z106">
+    <cfRule type="expression" dxfId="52" priority="34">
+      <formula>_xludf.isformula(A102:Z1121)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B101:Z101 A99:Z100">
+    <cfRule type="expression" dxfId="51" priority="35">
+      <formula>_xludf.isformula(A99:Z1116)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A108:W116">
+    <cfRule type="expression" dxfId="50" priority="36">
+      <formula>_xludf.isformula(D108:AC1128)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A81:Z81 K72:Z80 K83:Z91 B82:Z82">
+    <cfRule type="expression" dxfId="49" priority="38">
+      <formula>_xludf.isformula(A72:Z1084)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70:Z70">
+    <cfRule type="expression" dxfId="48" priority="39">
+      <formula>_xludf.isformula(A70:Z1078)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J25:Z25">
+    <cfRule type="expression" dxfId="46" priority="53">
+      <formula>_xludf.isformula(J25:AI1065)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J23:Z23 J50:Z55">
+    <cfRule type="expression" dxfId="45" priority="63">
+      <formula>_xludf.isformula(J23:AI1065)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16:Z16">
+    <cfRule type="expression" dxfId="44" priority="73">
+      <formula>_xludf.isformula(J16:AI1060)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="expression" dxfId="43" priority="96">
+      <formula>_xludf.isformula(A6:Z1003)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:H13 B40:H45 I40:I69">
+    <cfRule type="expression" dxfId="42" priority="98">
+      <formula>_xludf.isformula(A13:Z1060)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:H14">
+    <cfRule type="expression" dxfId="41" priority="101">
+      <formula>_xludf.isformula(A14:Z1060)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:H15">
+    <cfRule type="expression" dxfId="40" priority="104">
+      <formula>_xludf.isformula(A15:Z1060)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:H24">
+    <cfRule type="expression" dxfId="39" priority="110">
+      <formula>_xludf.isformula(A24:Z1065)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:H25">
+    <cfRule type="expression" dxfId="38" priority="117">
+      <formula>_xludf.isformula(A25:Z1065)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23:H23 B50:H55">
+    <cfRule type="expression" dxfId="37" priority="120">
+      <formula>_xludf.isformula(A23:Z1065)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:I6 B7:H12 I7:I37">
+    <cfRule type="expression" dxfId="36" priority="127">
+      <formula>_xludf.isformula(A6:Z1054)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A93:Z93">
+    <cfRule type="expression" dxfId="35" priority="130">
+      <formula>_xludf.isformula(A93:Z1106)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71:Z71">
+    <cfRule type="expression" dxfId="34" priority="131">
+      <formula>_xludf.isformula(A71:Z1081)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14:Z14 J46:Z46">
+    <cfRule type="expression" dxfId="33" priority="149">
+      <formula>_xludf.isformula(J14:AI1060)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15:Z15">
+    <cfRule type="expression" dxfId="32" priority="175">
+      <formula>_xludf.isformula(J15:AI1060)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A94:Z94">
+    <cfRule type="expression" dxfId="31" priority="185">
+      <formula>_xludf.isformula(A94:Z1109)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A92:Z92">
+    <cfRule type="expression" dxfId="30" priority="209">
+      <formula>_xludf.isformula(A92:Z1095)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:Z4">
+    <cfRule type="expression" dxfId="29" priority="268">
+      <formula>_xludf.isformula(A4:Z988)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J24:Z24">
+    <cfRule type="expression" dxfId="28" priority="269">
+      <formula>_xludf.isformula(J24:AI1065)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:H16">
+    <cfRule type="expression" dxfId="27" priority="270">
+      <formula>_xludf.isformula(A16:Z1060)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:Z5 J13:Z13 J39:Z45">
+    <cfRule type="expression" dxfId="26" priority="274">
+      <formula>_xludf.isformula(B5:AA1052)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J58:Z58 J26:Z37">
+    <cfRule type="expression" dxfId="25" priority="5">
+      <formula>_xludf.isformula(J26:AI1065)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J56:Z56">
+    <cfRule type="expression" dxfId="24" priority="6">
+      <formula>_xludf.isformula(J56:AI1097)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J49:Z49 J17:Z22">
+    <cfRule type="expression" dxfId="23" priority="7">
+      <formula>_xludf.isformula(J17:AI1060)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39">
+    <cfRule type="expression" dxfId="22" priority="8">
+      <formula>_xludf.isformula(A39:Z1035)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46:H46">
+    <cfRule type="expression" dxfId="21" priority="9">
+      <formula>_xludf.isformula(A46:Z1092)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47:H47">
+    <cfRule type="expression" dxfId="20" priority="10">
+      <formula>_xludf.isformula(A47:Z1092)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48:H48">
+    <cfRule type="expression" dxfId="19" priority="11">
+      <formula>_xludf.isformula(A48:Z1092)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:H57">
+    <cfRule type="expression" dxfId="18" priority="12">
+      <formula>_xludf.isformula(A57:Z1097)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58:H58 B26:H37">
+    <cfRule type="expression" dxfId="17" priority="13">
+      <formula>_xludf.isformula(A26:Z1065)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B56:H56">
+    <cfRule type="expression" dxfId="16" priority="14">
+      <formula>_xludf.isformula(A56:Z1097)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39:I39">
+    <cfRule type="expression" dxfId="15" priority="15">
+      <formula>_xludf.isformula(A39:Z1086)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J47:Z47">
+    <cfRule type="expression" dxfId="14" priority="16">
+      <formula>_xludf.isformula(J47:AI1092)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J48:Z48">
+    <cfRule type="expression" dxfId="13" priority="17">
+      <formula>_xludf.isformula(J48:AI1092)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J57:Z57">
+    <cfRule type="expression" dxfId="12" priority="18">
+      <formula>_xludf.isformula(J57:AI1097)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49:H49 B17:H22">
+    <cfRule type="expression" dxfId="11" priority="19">
+      <formula>_xludf.isformula(A17:Z1060)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:Z38">
+    <cfRule type="expression" dxfId="10" priority="21">
+      <formula>_xludf.isformula(A38:Z1084)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="expression" dxfId="9" priority="4">
+      <formula>_xludf.isformula(A5:Z1051)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82">
+    <cfRule type="expression" dxfId="8" priority="3">
+      <formula>_xludf.isformula(A82:Z1093)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A95:Z98">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>_xludf.isformula(A95:Z1111)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:A37">
+    <cfRule type="expression" dxfId="6" priority="305">
+      <formula>_xludf.isformula(Y7:XFD1055)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A101">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>_xludf.isformula(A101:Z1116)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:J91 B72:J80">
+    <cfRule type="expression" dxfId="4" priority="315">
+      <formula>_xludf.isformula(A72:Z1084)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6:Z12">
+    <cfRule type="expression" dxfId="3" priority="327">
+      <formula>_xludf.isformula(J6:AI1054)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J59:Z69">
+    <cfRule type="expression" dxfId="2" priority="329">
+      <formula>_xludf.isformula(J59:AI1097)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B59:H69">
+    <cfRule type="expression" dxfId="1" priority="330">
+      <formula>_xludf.isformula(A59:Z1097)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:A69">
+    <cfRule type="expression" dxfId="0" priority="331">
+      <formula>_xludf.isformula(Y40:XFD1087)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>